<commit_message>
reprovando por falta corretamente
</commit_message>
<xml_diff>
--- a/planilha/nova_planilha.xlsx
+++ b/planilha/nova_planilha.xlsx
@@ -417,7 +417,7 @@
         <v>Matricula</v>
       </c>
       <c r="B3" t="str">
-        <v>Aluno_Modificado</v>
+        <v>Aluno</v>
       </c>
       <c r="C3" t="str">
         <v>Faltas</v>
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="str">
-        <v>Eduardo_Modificado</v>
+        <v>Eduardo</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -456,6 +456,12 @@
       </c>
       <c r="F4">
         <v>61</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -463,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="str">
-        <v>Murilo_Modificado</v>
+        <v>Murilo</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -476,6 +482,12 @@
       </c>
       <c r="F5">
         <v>36</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -483,7 +495,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="str">
-        <v>Guilherme_Modificado</v>
+        <v>Guilherme</v>
       </c>
       <c r="C6">
         <v>19</v>
@@ -496,6 +508,12 @@
       </c>
       <c r="F6">
         <v>51</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -503,7 +521,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="str">
-        <v>Flavia _Modificado</v>
+        <v xml:space="preserve">Flavia </v>
       </c>
       <c r="C7">
         <v>23</v>
@@ -516,6 +534,12 @@
       </c>
       <c r="F7">
         <v>62</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="str">
-        <v>Ruan_Modificado</v>
+        <v>Ruan</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -536,6 +560,12 @@
       </c>
       <c r="F8">
         <v>41</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -543,7 +573,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="str">
-        <v>Arnando_Modificado</v>
+        <v>Arnando</v>
       </c>
       <c r="C9">
         <v>23</v>
@@ -556,6 +586,12 @@
       </c>
       <c r="F9">
         <v>77</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -563,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="str">
-        <v>Lucas_Modificado</v>
+        <v>Lucas</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -576,6 +612,12 @@
       </c>
       <c r="F10">
         <v>80</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -583,7 +625,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="str">
-        <v>Fabio_Modificado</v>
+        <v>Fabio</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -596,6 +638,12 @@
       </c>
       <c r="F11">
         <v>89</v>
+      </c>
+      <c r="G11" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -603,7 +651,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="str">
-        <v>Alisson_Modificado</v>
+        <v>Alisson</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -616,6 +664,12 @@
       </c>
       <c r="F12">
         <v>68</v>
+      </c>
+      <c r="G12" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -623,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="str">
-        <v>Felipe_Modificado</v>
+        <v>Felipe</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -636,6 +690,12 @@
       </c>
       <c r="F13">
         <v>85</v>
+      </c>
+      <c r="G13" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -643,7 +703,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="str">
-        <v>Rachel_Modificado</v>
+        <v>Rachel</v>
       </c>
       <c r="C14">
         <v>11</v>
@@ -656,6 +716,12 @@
       </c>
       <c r="F14">
         <v>39</v>
+      </c>
+      <c r="G14" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -663,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="str">
-        <v>Jouy_Modificado</v>
+        <v>Jouy</v>
       </c>
       <c r="C15">
         <v>13</v>
@@ -676,6 +742,12 @@
       </c>
       <c r="F15">
         <v>57</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -683,7 +755,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="str">
-        <v>François_Modificado</v>
+        <v>François</v>
       </c>
       <c r="C16">
         <v>19</v>
@@ -696,6 +768,12 @@
       </c>
       <c r="F16">
         <v>89</v>
+      </c>
+      <c r="G16" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -703,7 +781,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="str">
-        <v>Dâmaris_Modificado</v>
+        <v>Dâmaris</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -716,6 +794,12 @@
       </c>
       <c r="F17">
         <v>62</v>
+      </c>
+      <c r="G17" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -723,7 +807,7 @@
         <v>15</v>
       </c>
       <c r="B18" t="str">
-        <v>Leonardo_Modificado</v>
+        <v>Leonardo</v>
       </c>
       <c r="C18">
         <v>16</v>
@@ -736,6 +820,12 @@
       </c>
       <c r="F18">
         <v>32</v>
+      </c>
+      <c r="G18" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -743,7 +833,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="str">
-        <v>Guilherme _Modificado</v>
+        <v xml:space="preserve">Guilherme </v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -756,6 +846,12 @@
       </c>
       <c r="F19">
         <v>76</v>
+      </c>
+      <c r="G19" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -763,7 +859,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="str">
-        <v>Wesley_Modificado</v>
+        <v>Wesley</v>
       </c>
       <c r="C20">
         <v>16</v>
@@ -776,6 +872,12 @@
       </c>
       <c r="F20">
         <v>87</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -783,7 +885,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="str">
-        <v>Yuri_Modificado</v>
+        <v>Yuri</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -796,6 +898,12 @@
       </c>
       <c r="F21">
         <v>50</v>
+      </c>
+      <c r="G21" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -803,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="str">
-        <v>Kira_Modificado</v>
+        <v>Kira</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -816,6 +924,12 @@
       </c>
       <c r="F22">
         <v>48</v>
+      </c>
+      <c r="G22" t="str">
+        <v>Reprovado por Nota</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -823,7 +937,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="str">
-        <v>Cleici_Modificado</v>
+        <v>Cleici</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -836,6 +950,12 @@
       </c>
       <c r="F23">
         <v>92</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -843,7 +963,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="str">
-        <v>João Moacir_Modificado</v>
+        <v>João Moacir</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -856,6 +976,12 @@
       </c>
       <c r="F24">
         <v>98</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Reprovado por Falta</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -863,7 +989,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="str">
-        <v>Bruno_Modificado</v>
+        <v>Bruno</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -876,6 +1002,12 @@
       </c>
       <c r="F25">
         <v>100</v>
+      </c>
+      <c r="G25" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -883,7 +1015,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="str">
-        <v>Elcio_Modificado</v>
+        <v>Elcio</v>
       </c>
       <c r="C26">
         <v>9</v>
@@ -896,6 +1028,12 @@
       </c>
       <c r="F26">
         <v>75</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -903,7 +1041,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="str">
-        <v>Criscia_Modificado</v>
+        <v>Criscia</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -916,6 +1054,12 @@
       </c>
       <c r="F27">
         <v>84</v>
+      </c>
+      <c r="G27" t="str">
+        <v>Aprovado</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funções de reprovação por nota e calculo de media funcionando corretamente
</commit_message>
<xml_diff>
--- a/planilha/nova_planilha.xlsx
+++ b/planilha/nova_planilha.xlsx
@@ -458,10 +458,10 @@
         <v>61</v>
       </c>
       <c r="G4" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -484,10 +484,10 @@
         <v>36</v>
       </c>
       <c r="G5" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -562,10 +562,10 @@
         <v>41</v>
       </c>
       <c r="G8" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -614,10 +614,10 @@
         <v>80</v>
       </c>
       <c r="G10" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -666,10 +666,10 @@
         <v>68</v>
       </c>
       <c r="G12" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -692,10 +692,10 @@
         <v>85</v>
       </c>
       <c r="G13" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -718,10 +718,10 @@
         <v>39</v>
       </c>
       <c r="G14" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
@@ -744,10 +744,10 @@
         <v>57</v>
       </c>
       <c r="G15" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -796,10 +796,10 @@
         <v>62</v>
       </c>
       <c r="G17" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
@@ -848,10 +848,10 @@
         <v>76</v>
       </c>
       <c r="G19" t="str">
-        <v>Aprovado</v>
+        <v>Exame Final</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">

</xml_diff>